<commit_message>
Update example spreadsheet for control monotributistas
</commit_message>
<xml_diff>
--- a/planilla-control-monotributistas-ejemplo.xlsx
+++ b/planilla-control-monotributistas-ejemplo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t xml:space="preserve">CUIT_Representante</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">Descarga_MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descarga_MC_emitidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descarga_MC_recibidos</t>
   </si>
   <si>
     <t xml:space="preserve">Descarga_RCEL</t>
@@ -165,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,7 +184,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,10 +379,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,8 +428,14 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,34 +443,40 @@
         <v>20123456789</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>20987654321</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>45292</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>45657</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>45200</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>45689</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,34 +484,40 @@
         <v>20374730429</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>20374730429</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>45292</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>45657</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="n">
         <v>45200</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>45689</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>